<commit_message>
Minor fix update translation (Adres)
</commit_message>
<xml_diff>
--- a/doc/Translation-Therapy-Hessen_V2.xlsx
+++ b/doc/Translation-Therapy-Hessen_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Projects\Trunk\trnfrt.github.io\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821638D7-445B-4EAA-9A2D-81520202CE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D7C234-7CC1-411E-99B9-0C210D8FCB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="202">
   <si>
     <t>Turkish</t>
   </si>
@@ -629,6 +629,15 @@
   </si>
   <si>
     <t>Sosyal medya üzerinden bize ulaşın</t>
+  </si>
+  <si>
+    <t>address_title</t>
+  </si>
+  <si>
+    <t>Adres</t>
+  </si>
+  <si>
+    <t>Anschrift</t>
   </si>
 </sst>
 </file>
@@ -691,7 +700,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -759,11 +768,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -794,6 +814,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1014,12 +1037,12 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
+      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2514,6 +2537,29 @@
       </c>
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
+    </row>
+    <row r="64" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="E64" s="13" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$2, B64,Sheet2!B$3,C64,Sheet2!B$4)</f>
+        <v>"address_title": "Adres",</v>
+      </c>
+      <c r="F64" s="13" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$2, B64,Sheet2!B$3,D64,Sheet2!B$4)</f>
+        <v>"address_title": "Anschrift",</v>
+      </c>
+      <c r="G64" s="13" t="str">
+        <f>_xlfn.CONCAT(Sheet2!B$6,B64,Sheet2!B$7,B64,Sheet2!B$8)</f>
+        <v>$("[data-lang=address_title]").text(language.address_title);</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>